<commit_message>
Update test scenarios and add bonus API test
</commit_message>
<xml_diff>
--- a/testscen.xlsx
+++ b/testscen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mimon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DB0ACB-D3E6-48A1-896F-11A1CB125EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CFFAD2-4DAE-4A42-8325-222D8D1E4712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="915" windowWidth="17085" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Test Step</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Click Submit Reservation</t>
   </si>
   <si>
-    <t>Success dialog is displayed with text Thank you for reserving.</t>
-  </si>
-  <si>
     <t>TS-1 Book honeymoon plan</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Open Sign up page</t>
   </si>
   <si>
-    <t>Address; Tel (11 digits); Gender (male); DOB (YYYY-MM-DD)</t>
-  </si>
-  <si>
     <t>Click Sign up</t>
   </si>
   <si>
@@ -198,7 +192,34 @@
     <t>Redirected to MyPage</t>
   </si>
   <si>
-    <t>Icon image is visible on MyPage</t>
+    <t>Success page/message ‘Thank you for reserving.’</t>
+  </si>
+  <si>
+    <t>Address, Tel (11 digits), Gender (male), DoB (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Button = Sign up</t>
+  </si>
+  <si>
+    <t>Button = submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -  </t>
+  </si>
+  <si>
+    <t>Icon is saved/applied on MyPage (icon holder updated)</t>
+  </si>
+  <si>
+    <t>Navigate to MyPage (after Sign Up/Login)</t>
+  </si>
+  <si>
+    <t>MyPage is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Button = Login</t>
   </si>
 </sst>
 </file>
@@ -305,14 +326,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,23 +345,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -626,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E47"/>
+  <dimension ref="B3:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -644,446 +686,500 @@
   <sheetData>
     <row r="3" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
+      <c r="B11" s="19">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
+      <c r="B12" s="19">
         <v>2</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="19">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="19">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="19">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="19">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="19">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
+    <row r="26" spans="2:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="19">
+        <v>2</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B27" s="19">
         <v>3</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+      <c r="C27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="19">
         <v>4</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
+      <c r="C28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="19">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C31" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+    </row>
+    <row r="34" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B38" s="19">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="19">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E39" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="19">
+        <v>3</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="19">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B42" s="19">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C44" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+    </row>
+    <row r="47" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+    </row>
+    <row r="48" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+    </row>
+    <row r="50" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="19">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B53" s="19">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C18" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="63" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
+    <row r="54" spans="2:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="19">
         <v>3</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>4</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>5</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C29" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="D54" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="4">
-        <v>3</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="4">
-        <v>4</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C39" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="5"/>
-      <c r="C44" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
-        <v>2</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="4">
-        <v>3</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>49</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C39:E39"/>
+  <mergeCells count="17">
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C44:E44"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D35" r:id="rId1" tooltip="user/photo.png" display="https://file+.vscode-resource.vscode-cdn.net/c%3A/Users/mimon/.vscode/extensions/openai.chatgpt-0.4.71-win32-x64/webview/" xr:uid="{F0EB14B4-CA82-410A-87F9-C7FCC815F57A}"/>
+    <hyperlink ref="D40" r:id="rId1" tooltip="user/photo.png" display="https://file+.vscode-resource.vscode-cdn.net/c%3A/Users/mimon/.vscode/extensions/openai.chatgpt-0.4.71-win32-x64/webview/" xr:uid="{F0EB14B4-CA82-410A-87F9-C7FCC815F57A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>